<commit_message>
Back to improved Traffic Polygons. Distance EyePosition to Center View for zooming
</commit_message>
<xml_diff>
--- a/build/classes/airports/runways.xlsx
+++ b/build/classes/airports/runways.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\Master\TFM\World Wind\Simulator\src\airports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC20320B-AEE5-44B6-82CC-75EA99232627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7049817B-39CD-4DAB-817F-52625DB478A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
   <si>
     <t>Airport</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>355</t>
+  </si>
+  <si>
+    <t>Sign</t>
+  </si>
+  <si>
+    <t>06L/24R</t>
   </si>
 </sst>
 </file>
@@ -559,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,7 +651,9 @@
       <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="E3" s="8" t="s">
         <v>2</v>
       </c>
@@ -655,7 +663,9 @@
       <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="8"/>
+      <c r="H3" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="I3" s="8" t="s">
         <v>2</v>
       </c>
@@ -668,7 +678,9 @@
       <c r="L3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="8"/>
+      <c r="M3" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="N3" s="8" t="s">
         <v>2</v>
       </c>
@@ -678,7 +690,9 @@
       <c r="P3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="8"/>
+      <c r="Q3" s="6" t="s">
+        <v>22</v>
+      </c>
       <c r="R3" s="8" t="s">
         <v>2</v>
       </c>
@@ -824,66 +838,131 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E6">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6">
-        <v>54</v>
+        <v>17.690000000000001</v>
       </c>
       <c r="G6" s="7">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J6" s="12">
-        <v>25</v>
+        <v>4.32</v>
       </c>
       <c r="K6" s="7">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="L6" s="12">
-        <v>364</v>
+        <v>10</v>
       </c>
       <c r="M6" s="11" t="s">
         <v>14</v>
       </c>
       <c r="N6" s="12">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O6" s="12">
-        <v>53</v>
+        <v>18.34</v>
       </c>
       <c r="P6" s="7">
         <v>1</v>
       </c>
       <c r="Q6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R6" s="12">
+        <v>2</v>
+      </c>
+      <c r="S6" s="12">
+        <v>6.22</v>
+      </c>
+      <c r="T6" s="7">
+        <v>0</v>
+      </c>
+      <c r="U6" s="12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>54</v>
+      </c>
+      <c r="G7" s="7">
+        <v>42</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R6" s="12">
+      <c r="I7" s="12">
         <v>8</v>
       </c>
-      <c r="S6" s="12">
+      <c r="J7" s="12">
+        <v>25</v>
+      </c>
+      <c r="K7" s="7">
+        <v>13</v>
+      </c>
+      <c r="L7" s="12">
+        <v>364</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="12">
+        <v>42</v>
+      </c>
+      <c r="O7" s="12">
+        <v>53</v>
+      </c>
+      <c r="P7" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7" s="12">
+        <v>8</v>
+      </c>
+      <c r="S7" s="12">
         <v>24</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T7" s="7">
         <v>39</v>
       </c>
-      <c r="U6" s="12">
+      <c r="U7" s="12">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commands are now under Factory design pattern and moved to the SimulationEvents package
</commit_message>
<xml_diff>
--- a/build/classes/airports/runways.xlsx
+++ b/build/classes/airports/runways.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Desktop\Master\TFM\World Wind\Simulator\src\airports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7049817B-39CD-4DAB-817F-52625DB478A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6910808-8F39-4F53-8A09-DC359CBFE08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>Airport</t>
   </si>
@@ -90,13 +90,28 @@
     <t>Width (m)</t>
   </si>
   <si>
-    <t>355</t>
-  </si>
-  <si>
     <t>Sign</t>
   </si>
   <si>
     <t>06L/24R</t>
+  </si>
+  <si>
+    <t>LEBB</t>
+  </si>
+  <si>
+    <t>12/30</t>
+  </si>
+  <si>
+    <t>10/28</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>1169</t>
   </si>
 </sst>
 </file>
@@ -248,8 +263,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -259,16 +286,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -278,13 +295,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,69 +578,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="7"/>
-    <col min="2" max="2" width="8.7265625" style="9"/>
-    <col min="3" max="4" width="8.7265625" style="13"/>
-    <col min="7" max="7" width="8.7265625" style="7"/>
-    <col min="8" max="8" width="8.7265625" style="11"/>
-    <col min="11" max="11" width="8.7265625" style="7"/>
-    <col min="12" max="13" width="8.7265625" style="11"/>
-    <col min="16" max="16" width="8.7265625" style="7"/>
-    <col min="17" max="17" width="8.7265625" style="11"/>
-    <col min="20" max="20" width="8.7265625" style="7"/>
+    <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="2" max="2" width="8.7265625" style="6"/>
+    <col min="3" max="4" width="8.7265625" style="8"/>
+    <col min="7" max="7" width="8.7265625" style="4"/>
+    <col min="11" max="11" width="8.7265625" style="4"/>
+    <col min="16" max="16" width="8.7265625" style="4"/>
+    <col min="20" max="20" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A1" s="11"/>
-      <c r="B1" s="10"/>
-      <c r="C1" s="1" t="s">
+      <c r="A1"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="1" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="3"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="13"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="18" t="s">
+      <c r="A2"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="1" t="s">
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="17"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="9"/>
       <c r="M2" s="14" t="s">
         <v>7</v>
       </c>
@@ -642,81 +652,81 @@
       <c r="T2" s="16"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="4" t="s">
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="O3" s="4" t="s">
+      <c r="M3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="S3" s="4" t="s">
+      <c r="Q3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="T3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="19" t="s">
+      <c r="U3" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E4">
@@ -725,10 +735,10 @@
       <c r="F4">
         <v>17.27</v>
       </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>15</v>
       </c>
       <c r="I4">
@@ -737,13 +747,13 @@
       <c r="J4">
         <v>5.09</v>
       </c>
-      <c r="K4" s="7">
-        <v>0</v>
-      </c>
-      <c r="L4" s="12">
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4">
         <v>12</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" t="s">
         <v>14</v>
       </c>
       <c r="N4">
@@ -752,10 +762,10 @@
       <c r="O4">
         <v>18.559999999999999</v>
       </c>
-      <c r="P4" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="11" t="s">
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
         <v>15</v>
       </c>
       <c r="R4">
@@ -764,24 +774,24 @@
       <c r="S4">
         <v>5.68</v>
       </c>
-      <c r="T4" s="7">
-        <v>0</v>
-      </c>
-      <c r="U4" s="12">
+      <c r="T4" s="4">
+        <v>0</v>
+      </c>
+      <c r="U4">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E5">
@@ -790,63 +800,63 @@
       <c r="F5">
         <v>16.940000000000001</v>
       </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11" t="s">
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="12">
-        <v>2</v>
-      </c>
-      <c r="J5" s="12">
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
         <v>4.46</v>
       </c>
-      <c r="K5" s="7">
-        <v>0</v>
-      </c>
-      <c r="L5" s="12">
+      <c r="K5" s="4">
+        <v>0</v>
+      </c>
+      <c r="L5">
         <v>8</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="12">
+      <c r="N5">
         <v>41</v>
       </c>
-      <c r="O5" s="12">
+      <c r="O5">
         <v>17.53</v>
       </c>
-      <c r="P5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="11" t="s">
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
         <v>15</v>
       </c>
-      <c r="R5" s="12">
-        <v>2</v>
-      </c>
-      <c r="S5" s="12">
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
         <v>6.2</v>
       </c>
-      <c r="T5" s="7">
-        <v>0</v>
-      </c>
-      <c r="U5" s="12">
+      <c r="T5" s="4">
+        <v>0</v>
+      </c>
+      <c r="U5">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="B6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E6">
@@ -855,114 +865,244 @@
       <c r="F6">
         <v>17.690000000000001</v>
       </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="11" t="s">
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="12">
-        <v>2</v>
-      </c>
-      <c r="J6" s="12">
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
         <v>4.32</v>
       </c>
-      <c r="K6" s="7">
-        <v>0</v>
-      </c>
-      <c r="L6" s="12">
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>10</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="M6" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="12">
+      <c r="N6">
         <v>41</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O6">
         <v>18.34</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="4">
         <v>1</v>
       </c>
-      <c r="Q6" s="11" t="s">
+      <c r="Q6" t="s">
         <v>15</v>
       </c>
-      <c r="R6" s="12">
-        <v>2</v>
-      </c>
-      <c r="S6" s="12">
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
         <v>6.22</v>
       </c>
-      <c r="T6" s="7">
-        <v>0</v>
-      </c>
-      <c r="U6" s="12">
+      <c r="T6" s="4">
+        <v>0</v>
+      </c>
+      <c r="U6">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>43</v>
+      </c>
+      <c r="F7">
+        <v>18.38</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>55.5</v>
+      </c>
+      <c r="K7" s="4">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>128</v>
+      </c>
+      <c r="M7" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7">
+        <v>43</v>
+      </c>
+      <c r="O7">
+        <v>17.86</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <v>54.08</v>
+      </c>
+      <c r="T7" s="4">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>43</v>
+      </c>
+      <c r="F8">
+        <v>18.2</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>56.16</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>118</v>
+      </c>
+      <c r="M8" t="s">
+        <v>14</v>
+      </c>
+      <c r="N8">
+        <v>43</v>
+      </c>
+      <c r="O8">
+        <v>18.11</v>
+      </c>
+      <c r="P8" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>55.16</v>
+      </c>
+      <c r="T8" s="4">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="C9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E7">
+      <c r="E9">
         <v>42</v>
       </c>
-      <c r="F7">
+      <c r="F9">
         <v>54</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G9" s="4">
         <v>42</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H9" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I9">
         <v>8</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J9">
         <v>25</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K9" s="4">
         <v>13</v>
       </c>
-      <c r="L7" s="12">
-        <v>364</v>
-      </c>
-      <c r="M7" s="11" t="s">
+      <c r="L9">
+        <v>1200</v>
+      </c>
+      <c r="M9" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N9">
         <v>42</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O9">
         <v>53</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P9" s="4">
         <v>1</v>
       </c>
-      <c r="Q7" s="11" t="s">
+      <c r="Q9" t="s">
         <v>16</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R9">
         <v>8</v>
       </c>
-      <c r="S7" s="12">
+      <c r="S9">
         <v>24</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T9" s="4">
         <v>39</v>
       </c>
-      <c r="U7" s="12">
+      <c r="U9">
         <v>45</v>
       </c>
     </row>

</xml_diff>